<commit_message>
Update Run dataset code, fix bugs
</commit_message>
<xml_diff>
--- a/DRAM/Hudson_Bay.xlsx
+++ b/DRAM/Hudson_Bay.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ando/Documents/CGU/REU2020/An_version/PSO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ando/Documents/CGU/REU2020/Model-Fitting-on-Lotka-Volterra/Model-Fitting-on-Lotka-Volterra/DRAM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A01971D-6C0D-2D4F-AE0E-E42B0F3E6A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BBCCA0-B404-5645-954D-88D7F870153A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9740" yWindow="500" windowWidth="15780" windowHeight="14360" xr2:uid="{B074F861-2792-DC4B-866C-4954A1E5B217}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -415,7 +415,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1.847</v>
+        <v>1847</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -426,7 +426,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.8480000000000001</v>
+        <v>1848</v>
       </c>
       <c r="B3">
         <v>12</v>
@@ -437,7 +437,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.849</v>
+        <v>1849</v>
       </c>
       <c r="B4">
         <v>24</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.85</v>
+        <v>1850</v>
       </c>
       <c r="B5">
         <v>50</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1.851</v>
+        <v>1851</v>
       </c>
       <c r="B6">
         <v>80</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1.8520000000000001</v>
+        <v>1852</v>
       </c>
       <c r="B7">
         <v>80</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1.853</v>
+        <v>1853</v>
       </c>
       <c r="B8">
         <v>90</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1.8540000000000001</v>
+        <v>1854</v>
       </c>
       <c r="B9">
         <v>69</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1.855</v>
+        <v>1855</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -514,7 +514,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1.8560000000000001</v>
+        <v>1856</v>
       </c>
       <c r="B11">
         <v>93</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1.857</v>
+        <v>1857</v>
       </c>
       <c r="B12">
         <v>72</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1.8580000000000001</v>
+        <v>1858</v>
       </c>
       <c r="B13">
         <v>27</v>
@@ -547,7 +547,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1.859</v>
+        <v>1859</v>
       </c>
       <c r="B14">
         <v>14</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1.86</v>
+        <v>1860</v>
       </c>
       <c r="B15">
         <v>16</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1.861</v>
+        <v>1861</v>
       </c>
       <c r="B16">
         <v>38</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1.8620000000000001</v>
+        <v>1862</v>
       </c>
       <c r="B17">
         <v>5</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1.863</v>
+        <v>1863</v>
       </c>
       <c r="B18">
         <v>153</v>
@@ -602,7 +602,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1.8640000000000001</v>
+        <v>1864</v>
       </c>
       <c r="B19">
         <v>145</v>
@@ -613,7 +613,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1.865</v>
+        <v>1865</v>
       </c>
       <c r="B20">
         <v>106</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1.8660000000000001</v>
+        <v>1866</v>
       </c>
       <c r="B21">
         <v>46</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1.867</v>
+        <v>1867</v>
       </c>
       <c r="B22">
         <v>23</v>
@@ -646,7 +646,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1.8680000000000001</v>
+        <v>1868</v>
       </c>
       <c r="B23">
         <v>2</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1.869</v>
+        <v>1869</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1.87</v>
+        <v>1870</v>
       </c>
       <c r="B25">
         <v>8</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1.871</v>
+        <v>1871</v>
       </c>
       <c r="B26">
         <v>7</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1.8720000000000001</v>
+        <v>1872</v>
       </c>
       <c r="B27">
         <v>60</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>1.873</v>
+        <v>1873</v>
       </c>
       <c r="B28">
         <v>46</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1.8740000000000001</v>
+        <v>1874</v>
       </c>
       <c r="B29">
         <v>50</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>1.875</v>
+        <v>1875</v>
       </c>
       <c r="B30">
         <v>103</v>
@@ -734,7 +734,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1.8759999999999999</v>
+        <v>1876</v>
       </c>
       <c r="B31">
         <v>87</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1.877</v>
+        <v>1877</v>
       </c>
       <c r="B32">
         <v>68</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1.8779999999999999</v>
+        <v>1878</v>
       </c>
       <c r="B33">
         <v>17</v>
@@ -767,7 +767,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1.879</v>
+        <v>1879</v>
       </c>
       <c r="B34">
         <v>10</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1.88</v>
+        <v>1880</v>
       </c>
       <c r="B35">
         <v>17</v>
@@ -789,7 +789,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1.881</v>
+        <v>1881</v>
       </c>
       <c r="B36">
         <v>16</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1.8819999999999999</v>
+        <v>1882</v>
       </c>
       <c r="B37">
         <v>15</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1.883</v>
+        <v>1883</v>
       </c>
       <c r="B38">
         <v>46</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>1.8839999999999999</v>
+        <v>1884</v>
       </c>
       <c r="B39">
         <v>55</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1.885</v>
+        <v>1885</v>
       </c>
       <c r="B40">
         <v>137</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>1.8859999999999999</v>
+        <v>1886</v>
       </c>
       <c r="B41">
         <v>137</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>1.887</v>
+        <v>1887</v>
       </c>
       <c r="B42">
         <v>95</v>
@@ -866,7 +866,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>1.8879999999999999</v>
+        <v>1888</v>
       </c>
       <c r="B43">
         <v>37</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>1.889</v>
+        <v>1889</v>
       </c>
       <c r="B44">
         <v>22</v>
@@ -888,7 +888,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>1.89</v>
+        <v>1890</v>
       </c>
       <c r="B45">
         <v>50</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>1.891</v>
+        <v>1891</v>
       </c>
       <c r="B46">
         <v>54</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>1.8919999999999999</v>
+        <v>1892</v>
       </c>
       <c r="B47">
         <v>65</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>1.893</v>
+        <v>1893</v>
       </c>
       <c r="B48">
         <v>60</v>
@@ -932,7 +932,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>1.8939999999999999</v>
+        <v>1894</v>
       </c>
       <c r="B49">
         <v>81</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1.895</v>
+        <v>1895</v>
       </c>
       <c r="B50">
         <v>95</v>
@@ -954,7 +954,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>1.8959999999999999</v>
+        <v>1896</v>
       </c>
       <c r="B51">
         <v>56</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>1.897</v>
+        <v>1897</v>
       </c>
       <c r="B52">
         <v>18</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>1.8979999999999999</v>
+        <v>1898</v>
       </c>
       <c r="B53">
         <v>5</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>1.899</v>
+        <v>1899</v>
       </c>
       <c r="B54">
         <v>2</v>
@@ -998,7 +998,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>1.9</v>
+        <v>1900</v>
       </c>
       <c r="B55">
         <v>15</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>1.901</v>
+        <v>1901</v>
       </c>
       <c r="B56">
         <v>2</v>
@@ -1020,7 +1020,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>1.9019999999999999</v>
+        <v>1902</v>
       </c>
       <c r="B57">
         <v>6</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>1.903</v>
+        <v>1903</v>
       </c>
       <c r="B58">
         <v>45</v>

</xml_diff>